<commit_message>
Initial scenario runs on Macbook
</commit_message>
<xml_diff>
--- a/Data/MSM4PCoD_SimulationParameters.xlsx
+++ b/Data/MSM4PCoD_SimulationParameters.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EKJ/Documents/MSM4PCoD/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6254A70-2F82-0C49-992E-CD1580DBE18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC474CC6-1E13-4542-9E3B-DB84958C4017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11780" yWindow="1800" windowWidth="19080" windowHeight="14320" xr2:uid="{8ACACE82-7473-D842-90FC-39E203CC3EC4}"/>
+    <workbookView xWindow="7460" yWindow="2020" windowWidth="19080" windowHeight="14320" xr2:uid="{8ACACE82-7473-D842-90FC-39E203CC3EC4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
-  <si>
-    <t>A</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
   <si>
     <t>nyears</t>
   </si>
@@ -107,10 +105,121 @@
     <t>cr_int</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>pam_ecv</t>
+  </si>
+  <si>
+    <t>niter</t>
+  </si>
+  <si>
+    <t>nburnin</t>
+  </si>
+  <si>
+    <t>thin</t>
+  </si>
+  <si>
+    <t>chains</t>
+  </si>
+  <si>
+    <t>Number of simulations to run</t>
+  </si>
+  <si>
+    <t>Number of years to run each simulation</t>
+  </si>
+  <si>
+    <t>Connectivity between regions value (range 0 to 1)</t>
+  </si>
+  <si>
+    <t>Carrying capacity in region A during the first half of the simulation</t>
+  </si>
+  <si>
+    <t>Carrying capacity in region A during the second half of the simulation</t>
+  </si>
+  <si>
+    <t>Carrying capacity in region B during the first half of the simulation</t>
+  </si>
+  <si>
+    <t>Carrying capacity in region B during the second half of the simulation</t>
+  </si>
+  <si>
+    <t>nchains</t>
+  </si>
+  <si>
+    <t>Boolean, whether or not to simulate capture-recapture data collection</t>
+  </si>
+  <si>
+    <t>Interval between capture-recapture events</t>
+  </si>
+  <si>
+    <t>Year when capture-recapture effort begins</t>
+  </si>
+  <si>
+    <t>Year when capture-recapture effort ends</t>
+  </si>
+  <si>
+    <t>Probability of capture in capture-recapture surveys (constant, range 0 to 1)</t>
+  </si>
+  <si>
+    <t>Boolean, whether or not to simulate line-transect surveys</t>
+  </si>
+  <si>
+    <t>Year when line-transect effort begins</t>
+  </si>
+  <si>
+    <t>Year when line-transect effort ends</t>
+  </si>
+  <si>
+    <t>Interval between line-transect surveys</t>
+  </si>
+  <si>
+    <t>Expected CV of line-transect estimates of abundance</t>
+  </si>
+  <si>
+    <t>Boolean, whether or not to simulate passive acoustic monitoring surveys</t>
+  </si>
+  <si>
+    <t>Year when passive acoustic monitoring begins</t>
+  </si>
+  <si>
+    <t>Year when passive acoustic monitoring ends</t>
+  </si>
+  <si>
+    <t>Interval between passive acoustic monitoring estimates of abundance</t>
+  </si>
+  <si>
+    <t>Expected CV of passive acoustic monitoring estimates of abundance</t>
+  </si>
+  <si>
+    <t>Number of MCMC chains to run</t>
+  </si>
+  <si>
+    <t>Number of iterations per MCMC chain</t>
+  </si>
+  <si>
+    <t>Number of samples to discard as burnin (must be &lt; niter)</t>
+  </si>
+  <si>
+    <t>Thinning rate for MCMC chains</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>NULL_L</t>
+  </si>
+  <si>
+    <t>NULL_LC</t>
+  </si>
+  <si>
+    <t>NULL_LCP</t>
+  </si>
+  <si>
+    <t>D50_L</t>
+  </si>
+  <si>
+    <t>D50_LC</t>
+  </si>
+  <si>
+    <t>D50_LCP</t>
   </si>
 </sst>
 </file>
@@ -462,266 +571,941 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6D3D30-13D3-E447-8747-C0F158E1B478}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>90</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
+      </c>
+      <c r="G11">
+        <v>60</v>
+      </c>
+      <c r="H11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0.2</v>
+      </c>
+      <c r="C13">
+        <v>0.2</v>
+      </c>
+      <c r="D13">
+        <v>0.2</v>
+      </c>
+      <c r="E13">
+        <v>0.2</v>
+      </c>
+      <c r="F13">
+        <v>0.2</v>
+      </c>
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15">
+        <v>40</v>
+      </c>
+      <c r="H15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>60</v>
+      </c>
+      <c r="E16">
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>0.2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>0.6</v>
+      </c>
+      <c r="E18">
+        <v>0.6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18">
+        <v>0.6</v>
+      </c>
+      <c r="H18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>60</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="F23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23">
+        <v>0.35599999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>1000</v>
+      </c>
+      <c r="C25">
+        <v>50000</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25">
+        <v>10000</v>
+      </c>
+      <c r="F25">
+        <v>50000</v>
+      </c>
+      <c r="G25">
+        <v>10000</v>
+      </c>
+      <c r="H25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>900</v>
+      </c>
+      <c r="C26">
+        <v>40000</v>
+      </c>
+      <c r="D26">
+        <v>9000</v>
+      </c>
+      <c r="E26">
+        <v>9000</v>
+      </c>
+      <c r="F26">
+        <v>40000</v>
+      </c>
+      <c r="G26">
+        <v>9000</v>
+      </c>
+      <c r="H26">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EAEEE2-323C-4A46-9B4B-357C3A2B4CA6}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
-        <v>40</v>
-      </c>
-      <c r="C10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>60</v>
-      </c>
-      <c r="C11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>0.1</v>
-      </c>
-      <c r="C13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>40</v>
-      </c>
-      <c r="C15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16">
-        <v>60</v>
-      </c>
-      <c r="C16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>0.5</v>
-      </c>
-      <c r="C18">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Model runs and figures for end-May project update
</commit_message>
<xml_diff>
--- a/Data/MSM4PCoD_SimulationParameters.xlsx
+++ b/Data/MSM4PCoD_SimulationParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EKJ/Documents/MSM4PCoD/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC474CC6-1E13-4542-9E3B-DB84958C4017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07A5DFF-34BA-1041-A360-06446A7A53DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="2020" windowWidth="19080" windowHeight="14320" xr2:uid="{8ACACE82-7473-D842-90FC-39E203CC3EC4}"/>
+    <workbookView xWindow="17880" yWindow="2120" windowWidth="15160" windowHeight="13800" activeTab="1" xr2:uid="{8ACACE82-7473-D842-90FC-39E203CC3EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>nyears</t>
   </si>
@@ -93,9 +93,6 @@
     <t>pam_int</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>cr_start</t>
   </si>
   <si>
@@ -201,22 +198,7 @@
     <t>Thinning rate for MCMC chains</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>NULL_L</t>
-  </si>
-  <si>
-    <t>NULL_LC</t>
-  </si>
-  <si>
     <t>NULL_LCP</t>
-  </si>
-  <si>
-    <t>D50_L</t>
-  </si>
-  <si>
-    <t>D50_LC</t>
   </si>
   <si>
     <t>D50_LCP</t>
@@ -571,71 +553,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6D3D30-13D3-E447-8747-C0F158E1B478}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="E31:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -645,23 +594,8 @@
       <c r="C3">
         <v>100</v>
       </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -671,23 +605,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -697,23 +616,8 @@
       <c r="C5">
         <v>100</v>
       </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -723,23 +627,8 @@
       <c r="C6">
         <v>100</v>
       </c>
-      <c r="D6">
-        <v>100</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-      <c r="H6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -749,23 +638,8 @@
       <c r="C7">
         <v>100</v>
       </c>
-      <c r="D7">
-        <v>100</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -773,25 +647,10 @@
         <v>100</v>
       </c>
       <c r="C8">
-        <v>100</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-      <c r="H8">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -801,77 +660,32 @@
       <c r="C9" t="b">
         <v>1</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>40</v>
       </c>
-      <c r="D10">
-        <v>40</v>
-      </c>
-      <c r="E10">
-        <v>40</v>
-      </c>
-      <c r="F10">
-        <v>40</v>
-      </c>
-      <c r="G10">
-        <v>40</v>
-      </c>
-      <c r="H10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>60</v>
       </c>
-      <c r="D11">
-        <v>60</v>
-      </c>
-      <c r="E11">
-        <v>60</v>
-      </c>
-      <c r="F11">
-        <v>60</v>
-      </c>
-      <c r="G11">
-        <v>60</v>
-      </c>
-      <c r="H11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -879,23 +693,8 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -905,23 +704,8 @@
       <c r="C13">
         <v>0.2</v>
       </c>
-      <c r="D13">
-        <v>0.2</v>
-      </c>
-      <c r="E13">
-        <v>0.2</v>
-      </c>
-      <c r="F13">
-        <v>0.2</v>
-      </c>
-      <c r="G13">
-        <v>0.2</v>
-      </c>
-      <c r="H13">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -929,129 +713,54 @@
         <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15">
         <v>40</v>
       </c>
-      <c r="E15">
+      <c r="C15">
         <v>40</v>
       </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15">
-        <v>40</v>
-      </c>
-      <c r="H15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
-        <v>90</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16">
         <v>60</v>
       </c>
-      <c r="E16">
+      <c r="C16">
         <v>60</v>
       </c>
-      <c r="F16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16">
-        <v>60</v>
-      </c>
-      <c r="H16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17">
         <v>5</v>
       </c>
-      <c r="E17">
+      <c r="C17">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18">
-        <v>0.2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18">
         <v>0.6</v>
       </c>
-      <c r="E18">
+      <c r="C18">
         <v>0.6</v>
       </c>
-      <c r="F18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18">
-        <v>0.6</v>
-      </c>
-      <c r="H18">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1059,131 +768,56 @@
         <v>1</v>
       </c>
       <c r="C19" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20">
         <v>40</v>
       </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20">
+      <c r="C20">
         <v>40</v>
       </c>
-      <c r="F20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21">
         <v>60</v>
       </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21">
+      <c r="C21">
         <v>60</v>
       </c>
-      <c r="F21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23">
         <v>0.35599999999999998</v>
       </c>
-      <c r="F23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23">
+      <c r="C23">
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1191,97 +825,37 @@
       <c r="C24">
         <v>4</v>
       </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="F24">
-        <v>4</v>
-      </c>
-      <c r="G24">
-        <v>4</v>
-      </c>
-      <c r="H24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
-        <v>1000</v>
+        <v>50000</v>
       </c>
       <c r="C25">
         <v>50000</v>
       </c>
-      <c r="D25">
-        <v>10000</v>
-      </c>
-      <c r="E25">
-        <v>10000</v>
-      </c>
-      <c r="F25">
-        <v>50000</v>
-      </c>
-      <c r="G25">
-        <v>10000</v>
-      </c>
-      <c r="H25">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>900</v>
+        <v>40000</v>
       </c>
       <c r="C26">
         <v>40000</v>
       </c>
-      <c r="D26">
-        <v>9000</v>
-      </c>
-      <c r="E26">
-        <v>9000</v>
-      </c>
-      <c r="F26">
-        <v>40000</v>
-      </c>
-      <c r="G26">
-        <v>9000</v>
-      </c>
-      <c r="H26">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C27">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <v>10</v>
-      </c>
-      <c r="E27">
-        <v>10</v>
-      </c>
-      <c r="F27">
-        <v>10</v>
-      </c>
-      <c r="G27">
-        <v>10</v>
-      </c>
-      <c r="H27">
         <v>10</v>
       </c>
     </row>
@@ -1294,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EAEEE2-323C-4A46-9B4B-357C3A2B4CA6}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -1305,7 +879,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1313,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1321,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1329,7 +903,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1337,7 +911,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1345,7 +919,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1353,7 +927,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1361,31 +935,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1393,7 +967,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1401,7 +975,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1409,7 +983,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1417,7 +991,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1425,7 +999,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1433,7 +1007,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1441,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1449,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1457,7 +1031,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1465,47 +1039,47 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more scenarios follow convo with Cormac
</commit_message>
<xml_diff>
--- a/Data/MSM4PCoD_SimulationParameters.xlsx
+++ b/Data/MSM4PCoD_SimulationParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EKJ/Documents/MSM4PCoD/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07A5DFF-34BA-1041-A360-06446A7A53DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B6F88B-2C3D-7241-AB82-78877D07C649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="2120" windowWidth="15160" windowHeight="13800" activeTab="1" xr2:uid="{8ACACE82-7473-D842-90FC-39E203CC3EC4}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="37000" windowHeight="18000" xr2:uid="{8ACACE82-7473-D842-90FC-39E203CC3EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>nyears</t>
   </si>
@@ -202,6 +202,63 @@
   </si>
   <si>
     <t>D50_LCP</t>
+  </si>
+  <si>
+    <t>NULL_LCP_LowLTCV</t>
+  </si>
+  <si>
+    <t>D50_LCP_LowLTCV</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>D50_LCP_2023-06-27</t>
+  </si>
+  <si>
+    <t>NULL_LCP_2023-06-27</t>
+  </si>
+  <si>
+    <t>NULL_LCP_MidCval</t>
+  </si>
+  <si>
+    <t>D50_LCP_MidCval</t>
+  </si>
+  <si>
+    <t>D50_LCP_ZeroCval</t>
+  </si>
+  <si>
+    <t>NULL_LCP_ZeroCval</t>
+  </si>
+  <si>
+    <t>NULL_LCP_40Yrs</t>
+  </si>
+  <si>
+    <t>D50_LCP_40Yrs</t>
+  </si>
+  <si>
+    <t>NULL_LCP_LowPAMCV</t>
+  </si>
+  <si>
+    <t>D50_LCP_LowPAMCV</t>
+  </si>
+  <si>
+    <t>NULL_LCP_LowCVs</t>
+  </si>
+  <si>
+    <t>D50_LCP_LowCVs</t>
+  </si>
+  <si>
+    <t>D75_LCP_ZeroCval</t>
+  </si>
+  <si>
+    <t>D75_LCP_MidCval</t>
+  </si>
+  <si>
+    <t>NULL_LCP_HighCLowLTCV</t>
+  </si>
+  <si>
+    <t>D50_LCP_HighCLowLTCV</t>
   </si>
 </sst>
 </file>
@@ -553,38 +610,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6D3D30-13D3-E447-8747-C0F158E1B478}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="E31:F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>53</v>
       </c>
       <c r="C1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+      <c r="N2">
+        <v>100</v>
+      </c>
+      <c r="O2">
+        <v>100</v>
+      </c>
+      <c r="P2">
+        <v>100</v>
+      </c>
+      <c r="Q2">
+        <v>100</v>
+      </c>
+      <c r="R2">
+        <v>100</v>
+      </c>
+      <c r="S2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -594,8 +758,56 @@
       <c r="C3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>100</v>
+      </c>
+      <c r="O3">
+        <v>100</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+      <c r="R3">
+        <v>100</v>
+      </c>
+      <c r="S3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -605,8 +817,56 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+      <c r="K4">
+        <v>0.5</v>
+      </c>
+      <c r="L4">
+        <v>0.5</v>
+      </c>
+      <c r="M4">
+        <v>0.5</v>
+      </c>
+      <c r="N4">
+        <v>0.5</v>
+      </c>
+      <c r="O4">
+        <v>0.5</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>0.5</v>
+      </c>
+      <c r="S4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -616,8 +876,56 @@
       <c r="C5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <v>100</v>
+      </c>
+      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+      <c r="R5">
+        <v>100</v>
+      </c>
+      <c r="S5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -627,8 +935,56 @@
       <c r="C6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6">
+        <v>100</v>
+      </c>
+      <c r="N6">
+        <v>100</v>
+      </c>
+      <c r="O6">
+        <v>100</v>
+      </c>
+      <c r="P6">
+        <v>100</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+      <c r="R6">
+        <v>100</v>
+      </c>
+      <c r="S6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -638,8 +994,56 @@
       <c r="C7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="O7">
+        <v>100</v>
+      </c>
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="R7">
+        <v>100</v>
+      </c>
+      <c r="S7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -649,8 +1053,56 @@
       <c r="C8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>50</v>
+      </c>
+      <c r="K8">
+        <v>25</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>50</v>
+      </c>
+      <c r="N8">
+        <v>100</v>
+      </c>
+      <c r="O8">
+        <v>50</v>
+      </c>
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="Q8">
+        <v>50</v>
+      </c>
+      <c r="R8">
+        <v>100</v>
+      </c>
+      <c r="S8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -660,8 +1112,56 @@
       <c r="C9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -671,8 +1171,56 @@
       <c r="C10">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+      <c r="I10">
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <v>40</v>
+      </c>
+      <c r="L10">
+        <v>40</v>
+      </c>
+      <c r="M10">
+        <v>40</v>
+      </c>
+      <c r="N10">
+        <v>40</v>
+      </c>
+      <c r="O10">
+        <v>40</v>
+      </c>
+      <c r="P10">
+        <v>40</v>
+      </c>
+      <c r="Q10">
+        <v>40</v>
+      </c>
+      <c r="R10">
+        <v>40</v>
+      </c>
+      <c r="S10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -682,8 +1230,56 @@
       <c r="C11">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
+      </c>
+      <c r="G11">
+        <v>60</v>
+      </c>
+      <c r="H11">
+        <v>60</v>
+      </c>
+      <c r="I11">
+        <v>60</v>
+      </c>
+      <c r="J11">
+        <v>60</v>
+      </c>
+      <c r="K11">
+        <v>60</v>
+      </c>
+      <c r="L11">
+        <v>80</v>
+      </c>
+      <c r="M11">
+        <v>80</v>
+      </c>
+      <c r="N11">
+        <v>60</v>
+      </c>
+      <c r="O11">
+        <v>60</v>
+      </c>
+      <c r="P11">
+        <v>60</v>
+      </c>
+      <c r="Q11">
+        <v>60</v>
+      </c>
+      <c r="R11">
+        <v>60</v>
+      </c>
+      <c r="S11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -693,8 +1289,56 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -704,8 +1348,56 @@
       <c r="C13">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>0.2</v>
+      </c>
+      <c r="E13">
+        <v>0.2</v>
+      </c>
+      <c r="F13">
+        <v>0.2</v>
+      </c>
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13">
+        <v>0.2</v>
+      </c>
+      <c r="I13">
+        <v>0.2</v>
+      </c>
+      <c r="J13">
+        <v>0.2</v>
+      </c>
+      <c r="K13">
+        <v>0.2</v>
+      </c>
+      <c r="L13">
+        <v>0.2</v>
+      </c>
+      <c r="M13">
+        <v>0.2</v>
+      </c>
+      <c r="N13">
+        <v>0.2</v>
+      </c>
+      <c r="O13">
+        <v>0.2</v>
+      </c>
+      <c r="P13">
+        <v>0.2</v>
+      </c>
+      <c r="Q13">
+        <v>0.2</v>
+      </c>
+      <c r="R13">
+        <v>0.2</v>
+      </c>
+      <c r="S13">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -715,8 +1407,56 @@
       <c r="C14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="b">
+        <v>1</v>
+      </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -726,8 +1466,56 @@
       <c r="C15">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>40</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+      <c r="G15">
+        <v>40</v>
+      </c>
+      <c r="H15">
+        <v>40</v>
+      </c>
+      <c r="I15">
+        <v>40</v>
+      </c>
+      <c r="J15">
+        <v>40</v>
+      </c>
+      <c r="K15">
+        <v>40</v>
+      </c>
+      <c r="L15">
+        <v>40</v>
+      </c>
+      <c r="M15">
+        <v>40</v>
+      </c>
+      <c r="N15">
+        <v>40</v>
+      </c>
+      <c r="O15">
+        <v>40</v>
+      </c>
+      <c r="P15">
+        <v>40</v>
+      </c>
+      <c r="Q15">
+        <v>40</v>
+      </c>
+      <c r="R15">
+        <v>40</v>
+      </c>
+      <c r="S15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -737,8 +1525,56 @@
       <c r="C16">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>60</v>
+      </c>
+      <c r="E16">
+        <v>60</v>
+      </c>
+      <c r="F16">
+        <v>60</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>60</v>
+      </c>
+      <c r="I16">
+        <v>60</v>
+      </c>
+      <c r="J16">
+        <v>60</v>
+      </c>
+      <c r="K16">
+        <v>60</v>
+      </c>
+      <c r="L16">
+        <v>80</v>
+      </c>
+      <c r="M16">
+        <v>80</v>
+      </c>
+      <c r="N16">
+        <v>60</v>
+      </c>
+      <c r="O16">
+        <v>60</v>
+      </c>
+      <c r="P16">
+        <v>60</v>
+      </c>
+      <c r="Q16">
+        <v>60</v>
+      </c>
+      <c r="R16">
+        <v>60</v>
+      </c>
+      <c r="S16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -748,8 +1584,56 @@
       <c r="C17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <v>5</v>
+      </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <v>5</v>
+      </c>
+      <c r="R17">
+        <v>5</v>
+      </c>
+      <c r="S17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -759,8 +1643,56 @@
       <c r="C18">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>0.3</v>
+      </c>
+      <c r="E18">
+        <v>0.3</v>
+      </c>
+      <c r="F18">
+        <v>0.6</v>
+      </c>
+      <c r="G18">
+        <v>0.6</v>
+      </c>
+      <c r="H18">
+        <v>0.6</v>
+      </c>
+      <c r="I18">
+        <v>0.6</v>
+      </c>
+      <c r="J18">
+        <v>0.6</v>
+      </c>
+      <c r="K18">
+        <v>0.6</v>
+      </c>
+      <c r="L18">
+        <v>0.6</v>
+      </c>
+      <c r="M18">
+        <v>0.6</v>
+      </c>
+      <c r="N18">
+        <v>0.3</v>
+      </c>
+      <c r="O18">
+        <v>0.3</v>
+      </c>
+      <c r="P18">
+        <v>0.6</v>
+      </c>
+      <c r="Q18">
+        <v>0.6</v>
+      </c>
+      <c r="R18">
+        <v>0.3</v>
+      </c>
+      <c r="S18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -770,8 +1702,56 @@
       <c r="C19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="b">
+        <v>1</v>
+      </c>
+      <c r="R19" t="b">
+        <v>1</v>
+      </c>
+      <c r="S19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -781,8 +1761,56 @@
       <c r="C20">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>40</v>
+      </c>
+      <c r="G20">
+        <v>40</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+      <c r="I20">
+        <v>40</v>
+      </c>
+      <c r="J20">
+        <v>40</v>
+      </c>
+      <c r="K20">
+        <v>40</v>
+      </c>
+      <c r="L20">
+        <v>40</v>
+      </c>
+      <c r="M20">
+        <v>40</v>
+      </c>
+      <c r="N20">
+        <v>40</v>
+      </c>
+      <c r="O20">
+        <v>40</v>
+      </c>
+      <c r="P20">
+        <v>40</v>
+      </c>
+      <c r="Q20">
+        <v>40</v>
+      </c>
+      <c r="R20">
+        <v>40</v>
+      </c>
+      <c r="S20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -792,8 +1820,56 @@
       <c r="C21">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <v>60</v>
+      </c>
+      <c r="G21">
+        <v>60</v>
+      </c>
+      <c r="H21">
+        <v>60</v>
+      </c>
+      <c r="I21">
+        <v>60</v>
+      </c>
+      <c r="J21">
+        <v>60</v>
+      </c>
+      <c r="K21">
+        <v>60</v>
+      </c>
+      <c r="L21">
+        <v>80</v>
+      </c>
+      <c r="M21">
+        <v>80</v>
+      </c>
+      <c r="N21">
+        <v>60</v>
+      </c>
+      <c r="O21">
+        <v>60</v>
+      </c>
+      <c r="P21">
+        <v>60</v>
+      </c>
+      <c r="Q21">
+        <v>60</v>
+      </c>
+      <c r="R21">
+        <v>60</v>
+      </c>
+      <c r="S21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -803,8 +1879,56 @@
       <c r="C22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -814,8 +1938,56 @@
       <c r="C23">
         <v>0.35599999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="E23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="F23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="G23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="H23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="I23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="J23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="K23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="L23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="M23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="N23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="O23">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="P23">
+        <v>0.18</v>
+      </c>
+      <c r="Q23">
+        <v>0.18</v>
+      </c>
+      <c r="R23">
+        <v>0.18</v>
+      </c>
+      <c r="S23">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -825,8 +1997,56 @@
       <c r="C24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>4</v>
+      </c>
+      <c r="P24">
+        <v>4</v>
+      </c>
+      <c r="Q24">
+        <v>4</v>
+      </c>
+      <c r="R24">
+        <v>4</v>
+      </c>
+      <c r="S24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -836,8 +2056,56 @@
       <c r="C25">
         <v>50000</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>50000</v>
+      </c>
+      <c r="E25">
+        <v>50000</v>
+      </c>
+      <c r="F25">
+        <v>50000</v>
+      </c>
+      <c r="G25">
+        <v>50000</v>
+      </c>
+      <c r="H25">
+        <v>50000</v>
+      </c>
+      <c r="I25">
+        <v>50000</v>
+      </c>
+      <c r="J25">
+        <v>50000</v>
+      </c>
+      <c r="K25">
+        <v>50000</v>
+      </c>
+      <c r="L25">
+        <v>50000</v>
+      </c>
+      <c r="M25">
+        <v>50000</v>
+      </c>
+      <c r="N25">
+        <v>50000</v>
+      </c>
+      <c r="O25">
+        <v>50000</v>
+      </c>
+      <c r="P25">
+        <v>50000</v>
+      </c>
+      <c r="Q25">
+        <v>50000</v>
+      </c>
+      <c r="R25">
+        <v>50000</v>
+      </c>
+      <c r="S25">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -847,8 +2115,56 @@
       <c r="C26">
         <v>40000</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>40000</v>
+      </c>
+      <c r="E26">
+        <v>40000</v>
+      </c>
+      <c r="F26">
+        <v>40000</v>
+      </c>
+      <c r="G26">
+        <v>40000</v>
+      </c>
+      <c r="H26">
+        <v>40000</v>
+      </c>
+      <c r="I26">
+        <v>40000</v>
+      </c>
+      <c r="J26">
+        <v>40000</v>
+      </c>
+      <c r="K26">
+        <v>40000</v>
+      </c>
+      <c r="L26">
+        <v>40000</v>
+      </c>
+      <c r="M26">
+        <v>40000</v>
+      </c>
+      <c r="N26">
+        <v>40000</v>
+      </c>
+      <c r="O26">
+        <v>40000</v>
+      </c>
+      <c r="P26">
+        <v>40000</v>
+      </c>
+      <c r="Q26">
+        <v>40000</v>
+      </c>
+      <c r="R26">
+        <v>40000</v>
+      </c>
+      <c r="S26">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -857,6 +2173,71 @@
       </c>
       <c r="C27">
         <v>10</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="J27">
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <v>10</v>
+      </c>
+      <c r="L27">
+        <v>10</v>
+      </c>
+      <c r="M27">
+        <v>10</v>
+      </c>
+      <c r="N27">
+        <v>10</v>
+      </c>
+      <c r="O27">
+        <v>10</v>
+      </c>
+      <c r="P27">
+        <v>10</v>
+      </c>
+      <c r="Q27">
+        <v>10</v>
+      </c>
+      <c r="R27">
+        <v>10</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +2249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EAEEE2-323C-4A46-9B4B-357C3A2B4CA6}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>

</xml_diff>